<commit_message>
update exercise attribute names
</commit_message>
<xml_diff>
--- a/ids720_specific/class_schedule_720_xlsx.xlsx
+++ b/ids720_specific/class_schedule_720_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids720_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B37EC5-61A1-8E41-B831-82BA031323D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5D8452-AC77-FE4E-A7BC-820937D2FDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -428,8 +428,7 @@
   <si>
     <t>- Data Cleaning  from `Identifying Problems &lt;../notebooks/class_3/week_3/20_cleaning_identifying.html&gt;`_ through `Cleaning Data Types &lt;../notebooks/class_3/week_3/33_cleaning_datatypes.html&gt;`_
 - `f-strings &lt;../notebooks/other/fstrings.html&gt;`_
-- `Python Strings (string section only!) &lt;https://realpython.com/python-data-types/#strings&gt;`_
-- `Regex &lt;https://realpython.com/regex-python/&gt;`_</t>
+- `Datacamp Class "Regular Expressions for Pattern Matching," Chapter 3 (Introduction to regular expressions) &lt;https://campus.datacamp.com/courses/regular-expressions-in-python/basic-concepts-of-string-manipulation?ex=1&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -837,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
swap after break readings
</commit_message>
<xml_diff>
--- a/ids720_specific/class_schedule_720_xlsx.xlsx
+++ b/ids720_specific/class_schedule_720_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids720_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360F065D-8F93-F346-94D5-C065AB7C6D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFE014C-8CA4-3E47-B0B5-E906777F4616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="2220" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -233,10 +233,6 @@
 - `Opioid Project &lt;https://github.com/nickeubank/practicaldatascience_book/blob/main/ids720_specific/opioids/PDS_ProjectSummary.pdf&gt;`_</t>
   </si>
   <si>
-    <t>- Defensive Programming: from `first reading &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/defensive_programming.html&gt;`_ through `Iceberg Principle &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/iceberg_principle.html&gt;`_
-- `Groupby &lt;../notebooks/class_3/week_4/20_grouping.html&gt;`_</t>
-  </si>
-  <si>
     <t>- Wes McKinney's *Python for Data Analysis*, Third Edition, Chapter 8, Section 3. Available `online through duke library free &lt;https://learning.oreilly.com/library/view/python-for-data/9781098104023/ch08.html#prep_reshape&gt;`_
 - `Tidy Data Format: the goal of reshaping &lt;http://vita.had.co.nz/papers/tidy-data.html&gt;`_
 - `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_</t>
@@ -270,12 +266,6 @@
     <t>- Read all readings under the Statistical Modelling heading, starting with `Inference and Prediction &lt;../notebooks/class_5/week_3/20_inference_v_prediction.html&gt;`_ through `Beyond the Basic Model &lt;../notebooks/class_5/week_3/40_linear_regression_extensions&gt;`_</t>
   </si>
   <si>
-    <t>- `Workflow Management &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/workflow.html&gt;`_
-- `Backwards Design &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/backwards_design.html&gt;`_
-- `Getting Help &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/getting_help.html&gt;`_
-- `Code Reviews &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/pr_review.html&gt;`_</t>
-  </si>
-  <si>
     <t>Tues, Aug 26</t>
   </si>
   <si>
@@ -429,6 +419,15 @@
   <si>
     <t>- `Dask &lt;exercises/exercise_dask_realdata.html&gt;`_
 - `More dask (optional) &lt;exercises/exercise_dask.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Groupby &lt;../notebooks/class_3/week_4/20_grouping.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Defensive Programming: from `first reading &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/defensive_programming.html&gt;`_ through `Iceberg Principle &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/iceberg_principle.html&gt;`_
+- `Workflow Management &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/workflow.html&gt;`_
+- `Getting Help &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/getting_help.html&gt;`_
+- `Code Reviews &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/pr_review.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -836,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -864,7 +863,7 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
@@ -876,7 +875,7 @@
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>16</v>
@@ -885,12 +884,12 @@
         <v>28</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>31</v>
@@ -899,12 +898,12 @@
         <v>30</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
@@ -913,12 +912,12 @@
         <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>34</v>
@@ -927,12 +926,12 @@
         <v>35</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>6</v>
@@ -941,12 +940,12 @@
         <v>36</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>18</v>
@@ -955,12 +954,12 @@
         <v>37</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
@@ -969,12 +968,12 @@
         <v>38</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>8</v>
@@ -983,40 +982,40 @@
         <v>39</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>22</v>
@@ -1025,12 +1024,12 @@
         <v>40</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>22</v>
@@ -1039,12 +1038,12 @@
         <v>41</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>21</v>
@@ -1053,12 +1052,12 @@
         <v>42</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -1066,145 +1065,145 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>43</v>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="D25" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>